<commit_message>
chore(quotation): fill completion totals cells
</commit_message>
<xml_diff>
--- a/backend/templates/quotation/美菱改模完工确认单.xlsx
+++ b/backend/templates/quotation/美菱改模完工确认单.xlsx
@@ -5,15 +5,15 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changun/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changun/work/jiuhuan/backend/templates/quotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A797817-237E-F84E-93FD-8DCDCD21A8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F640D0AA-DC0C-A945-B3BC-2801D545616D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="40960" windowHeight="22420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="改模报价" sheetId="1" r:id="rId1"/>
+    <sheet name="完工确认单" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -214,6 +214,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="#,##0.00_ "/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -547,7 +550,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -572,13 +575,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -594,6 +600,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -952,15 +961,15 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" customWidth="1"/>
@@ -969,17 +978,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
     </row>
     <row r="2" spans="1:9" ht="25" customHeight="1">
       <c r="A2" s="9" t="s">
@@ -994,37 +1003,37 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="8"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="20" customHeight="1">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:9" ht="21" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="10"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:9" ht="20" customHeight="1">
       <c r="A5" s="9" t="s">
@@ -1037,9 +1046,9 @@
       <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="24"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:9" ht="20" customHeight="1">
       <c r="A6" s="9" t="s">
@@ -1052,7 +1061,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
-      <c r="I6" s="8"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1">
       <c r="A7" s="9" t="s">
@@ -1080,12 +1089,12 @@
     <row r="8" spans="1:9" ht="20" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
       <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9" ht="20" customHeight="1">
@@ -1095,8 +1104,8 @@
       <c r="D9" s="10"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
       <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9" ht="20" customHeight="1">
@@ -1106,8 +1115,8 @@
       <c r="D10" s="10"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
       <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:9" ht="20" customHeight="1">
@@ -1117,8 +1126,8 @@
       <c r="D11" s="10"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="8"/>
     </row>
     <row r="12" spans="1:9" ht="20" customHeight="1">
@@ -1128,8 +1137,8 @@
       <c r="D12" s="10"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
       <c r="I12" s="8"/>
     </row>
     <row r="13" spans="1:9" ht="20" customHeight="1">
@@ -1166,8 +1175,8 @@
         <v>20</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
       <c r="I14" s="8"/>
     </row>
     <row r="15" spans="1:9" ht="20" customHeight="1">
@@ -1181,8 +1190,8 @@
         <v>22</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
       <c r="I15" s="8"/>
     </row>
     <row r="16" spans="1:9" ht="20" customHeight="1">
@@ -1196,8 +1205,8 @@
         <v>24</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
       <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:9" ht="20" customHeight="1">
@@ -1211,8 +1220,8 @@
         <v>26</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:9" ht="20" customHeight="1">
@@ -1226,8 +1235,8 @@
         <v>26</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
       <c r="I18" s="8"/>
     </row>
     <row r="19" spans="1:9" ht="20" customHeight="1">
@@ -1241,8 +1250,8 @@
         <v>29</v>
       </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="8"/>
     </row>
     <row r="20" spans="1:9" ht="20" customHeight="1">
@@ -1256,8 +1265,8 @@
         <v>31</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="20" customHeight="1">
@@ -1271,8 +1280,8 @@
         <v>33</v>
       </c>
       <c r="F21" s="4"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
       <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:9" ht="20" customHeight="1">
@@ -1286,8 +1295,8 @@
         <v>20</v>
       </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
       <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9" ht="20" customHeight="1">
@@ -1301,8 +1310,8 @@
         <v>36</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
       <c r="I23" s="8"/>
     </row>
     <row r="24" spans="1:9" ht="20" customHeight="1">
@@ -1316,8 +1325,8 @@
       <c r="F24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
       <c r="I24" s="8"/>
     </row>
     <row r="25" spans="1:9" ht="20" customHeight="1">
@@ -1333,8 +1342,8 @@
       <c r="F25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
       <c r="I25" s="8"/>
     </row>
     <row r="26" spans="1:9" ht="27" customHeight="1">
@@ -1351,21 +1360,21 @@
       <c r="G26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H26" s="10"/>
+      <c r="H26" s="17"/>
       <c r="I26" s="8"/>
     </row>
     <row r="27" spans="1:9" ht="24.5" customHeight="1">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="16"/>
     </row>
     <row r="28" spans="1:9" ht="20" customHeight="1">
       <c r="A28" s="9" t="s">
@@ -1380,20 +1389,20 @@
       <c r="H28" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I28" s="8"/>
+      <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9" ht="20" customHeight="1">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="16"/>
     </row>
     <row r="30" spans="1:9" ht="18" customHeight="1">
       <c r="A30" s="9" t="s">
@@ -1408,7 +1417,7 @@
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
-      <c r="I30" s="8"/>
+      <c r="I30" s="11"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1">
       <c r="A31" s="9" t="s">
@@ -1423,7 +1432,7 @@
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
-      <c r="I31" s="8"/>
+      <c r="I31" s="11"/>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1">
       <c r="A32" s="9"/>
@@ -1436,20 +1445,20 @@
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
-      <c r="I32" s="8"/>
+      <c r="I32" s="11"/>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1">
       <c r="A33" s="9"/>
       <c r="B33" s="10"/>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:9" ht="20" customHeight="1">
       <c r="A34" s="9" t="s">
@@ -1466,7 +1475,7 @@
         <v>54</v>
       </c>
       <c r="H34" s="10"/>
-      <c r="I34" s="8"/>
+      <c r="I34" s="11"/>
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1">
       <c r="A35" s="5"/>

</xml_diff>

<commit_message>
chore(ui): adjust mobile query actions spacing
</commit_message>
<xml_diff>
--- a/backend/templates/quotation/美菱改模完工确认单.xlsx
+++ b/backend/templates/quotation/美菱改模完工确认单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changun/work/jiuhuan/backend/templates/quotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F640D0AA-DC0C-A945-B3BC-2801D545616D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D491D3A-C1FB-CE4C-80C2-E0B8264FD70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="40960" windowHeight="22420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,7 +550,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -566,6 +566,78 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -573,18 +645,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -593,65 +653,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,7 +964,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -978,381 +981,381 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" ht="25" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="20" customHeight="1">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" ht="21" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" ht="20" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="26"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:9" ht="20" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="8"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="34"/>
     </row>
     <row r="9" spans="1:9" ht="20" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="8"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="34"/>
     </row>
     <row r="10" spans="1:9" ht="20" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="8"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="34"/>
     </row>
     <row r="11" spans="1:9" ht="20" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="8"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="34"/>
     </row>
     <row r="12" spans="1:9" ht="20" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="8"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="34"/>
     </row>
     <row r="13" spans="1:9" ht="20" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="10"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="20" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="10"/>
+      <c r="D14" s="9"/>
       <c r="E14" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="8"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="34"/>
     </row>
     <row r="15" spans="1:9" ht="20" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="8"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="34"/>
     </row>
     <row r="16" spans="1:9" ht="20" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="8"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="34"/>
     </row>
     <row r="17" spans="1:9" ht="20" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="8"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="34"/>
     </row>
     <row r="18" spans="1:9" ht="20" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10" t="s">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="8"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="34"/>
     </row>
     <row r="19" spans="1:9" ht="20" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="8"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="34"/>
     </row>
     <row r="20" spans="1:9" ht="20" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="8"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="34"/>
     </row>
     <row r="21" spans="1:9" ht="20" customHeight="1">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="4" t="s">
         <v>33</v>
       </c>
       <c r="F21" s="4"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="8"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="34"/>
     </row>
     <row r="22" spans="1:9" ht="20" customHeight="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="9"/>
       <c r="E22" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="8"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="34"/>
     </row>
     <row r="23" spans="1:9" ht="20" customHeight="1">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="10"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="8"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="34"/>
     </row>
     <row r="24" spans="1:9" ht="20" customHeight="1">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="8"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="25"/>
     </row>
     <row r="25" spans="1:9" ht="20" customHeight="1">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="8"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="25"/>
     </row>
     <row r="26" spans="1:9" ht="27" customHeight="1">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
       <c r="E26" s="4" t="s">
         <v>10</v>
       </c>
@@ -1360,198 +1363,136 @@
       <c r="G26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H26" s="17"/>
-      <c r="I26" s="8"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="25"/>
     </row>
     <row r="27" spans="1:9" ht="24.5" customHeight="1">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="16"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="28"/>
     </row>
     <row r="28" spans="1:9" ht="20" customHeight="1">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="I28" s="11"/>
+      <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" ht="20" customHeight="1">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="16"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="28"/>
     </row>
     <row r="30" spans="1:9" ht="18" customHeight="1">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
       <c r="F30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="11"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
       <c r="F31" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="11"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
       <c r="F32" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="11"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="12" t="s">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="13"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="33"/>
     </row>
     <row r="34" spans="1:9" ht="20" customHeight="1">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10" t="s">
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="11"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="7"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="G35:I35"/>
@@ -1568,6 +1509,68 @@
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="A29:I29"/>
     <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>